<commit_message>
Scripts y bd con errores
</commit_message>
<xml_diff>
--- a/bd_pruebas.xlsx
+++ b/bd_pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramir\OneDrive\Escritorio\Universidad\Ingesoft 2\Proyecto\ingesoft2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3639B27-7009-4BC4-9310-5FE90F75AC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D4A877-8C82-4A44-BF3C-511CB28A3852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
   <si>
     <t>cedula</t>
   </si>
@@ -607,7 +607,7 @@
   <dimension ref="A1:G353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,17 +646,9 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
       </c>
       <c r="G2">
         <v>671</v>
@@ -675,9 +667,7 @@
       <c r="D3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" t="s">
         <v>62</v>
       </c>
@@ -712,9 +702,7 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" t="s">
         <v>34</v>
       </c>
@@ -723,9 +711,6 @@
       </c>
       <c r="F5" t="s">
         <v>69</v>
-      </c>
-      <c r="G5">
-        <v>579</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ni idea, está acabado????
* Scripts y bd con errores

* Bases de datos direcciones

* Script en R

* Limpiando archivos

* no sé

* proyecto casi terminado

* proyecto casi terminado

* proyecto acabado(??

---------

Co-authored-by: ARJ48 <japiedrahitam@upn.edu.co>
</commit_message>
<xml_diff>
--- a/bd_pruebas.xlsx
+++ b/bd_pruebas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramir\OneDrive\Escritorio\Universidad\Ingesoft 2\Proyecto\ingesoft2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D4A877-8C82-4A44-BF3C-511CB28A3852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B04E797-5A73-4DEB-B541-269EE52B41B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
   <si>
     <t>cedula</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Oscar</t>
   </si>
   <si>
-    <t>Manuel</t>
-  </si>
-  <si>
     <t>Claudia</t>
   </si>
   <si>
@@ -273,6 +270,93 @@
   </si>
   <si>
     <t>Maria Gloria</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>rsnaith0@symantec.com</t>
+  </si>
+  <si>
+    <t>saucoate1@pcworld.com</t>
+  </si>
+  <si>
+    <t>dcarefull2@wikimedia.org</t>
+  </si>
+  <si>
+    <t>mtrathan3@ca.gov</t>
+  </si>
+  <si>
+    <t>sluis4@vk.com</t>
+  </si>
+  <si>
+    <t>saggas5@dagondesign.com</t>
+  </si>
+  <si>
+    <t>apuncher6@linkedin.com</t>
+  </si>
+  <si>
+    <t>dmarkovich7@trellian.com</t>
+  </si>
+  <si>
+    <t>lescott8@timesonline.co.uk</t>
+  </si>
+  <si>
+    <t>koharney9@businessinsider.com</t>
+  </si>
+  <si>
+    <t>ssmailsa@livejournal.com</t>
+  </si>
+  <si>
+    <t>sgatheralb@prweb.com</t>
+  </si>
+  <si>
+    <t>glownesc@nasa.gov</t>
+  </si>
+  <si>
+    <t>mgronousd@guardian.co.uk</t>
+  </si>
+  <si>
+    <t>manscotte@sina.com.cn</t>
+  </si>
+  <si>
+    <t>vtinkerf@people.com.cn</t>
+  </si>
+  <si>
+    <t>cbertrandg@nymag.com</t>
+  </si>
+  <si>
+    <t>knutkinh@google.com</t>
+  </si>
+  <si>
+    <t>lkippeni@bing.com</t>
+  </si>
+  <si>
+    <t>amcmillianj@constantcontact.com</t>
+  </si>
+  <si>
+    <t>ehebbesk@google.com.hk</t>
+  </si>
+  <si>
+    <t>pvardiel@stumbleupon.com</t>
+  </si>
+  <si>
+    <t>hgobolosm@mozilla.org</t>
+  </si>
+  <si>
+    <t>nmallenn@theatlantic.com</t>
+  </si>
+  <si>
+    <t>tthwaiteo@irs.gov</t>
+  </si>
+  <si>
+    <t>enursep@over-blog.com</t>
+  </si>
+  <si>
+    <t>mferneq@webs.com</t>
+  </si>
+  <si>
+    <t>Jorge Manuel</t>
   </si>
 </sst>
 </file>
@@ -321,9 +405,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G353"/>
+  <dimension ref="A1:H353"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,21 +702,21 @@
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>74</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -638,9 +724,12 @@
       <c r="G1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1111</v>
       </c>
       <c r="B2" t="s">
@@ -648,14 +737,17 @@
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2">
         <v>671</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>2222</v>
       </c>
       <c r="B3" t="s">
@@ -665,38 +757,44 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3">
         <v>202</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="H3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>3333</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4">
         <v>991</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="H4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>4444</v>
       </c>
       <c r="B5" t="s">
@@ -704,17 +802,20 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
+        <v>68</v>
+      </c>
+      <c r="H5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>5555</v>
       </c>
       <c r="B6" t="s">
@@ -724,17 +825,20 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G6">
         <v>967</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="H6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>6666</v>
       </c>
       <c r="B7" t="s">
@@ -744,20 +848,23 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7">
         <v>244</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="H7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>7777</v>
       </c>
       <c r="B8" t="s">
@@ -767,60 +874,67 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G8">
         <v>413</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="H8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>8888</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="C9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G9">
         <v>101</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="H9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>9999</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G10">
         <v>355</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="H10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>1010</v>
       </c>
       <c r="B11" t="s">
@@ -830,183 +944,210 @@
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11">
         <v>304</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="H11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>1011</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G12">
         <v>387</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="H12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>1012</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G13">
         <v>137</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="H13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>1013</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G14">
         <v>792</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="H14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
         <v>1014</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1015</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>1015</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16">
         <v>412</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="H16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
         <v>1016</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18">
+        <v>64</v>
+      </c>
+      <c r="H17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
         <v>1017</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18">
         <v>206</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="H18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>1018</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G19">
         <v>429</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="H19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>1019</v>
       </c>
       <c r="B20" t="s">
@@ -1014,91 +1155,109 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G20">
         <v>795</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="H20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
         <v>1020</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
         <v>30</v>
       </c>
-      <c r="D21" t="s">
-        <v>31</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G21">
         <v>163</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="H21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
         <v>1111</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G22">
         <v>671</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="H22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
         <v>1111</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="F23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
         <v>1111</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G24">
         <v>671</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="H24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
         <v>2222</v>
       </c>
       <c r="B25" t="s">
@@ -1108,86 +1267,96 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G25">
         <v>202</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="H25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
         <v>4444</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G26">
         <v>579</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="H26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
         <v>8888</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G27">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="H27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
         <v>1011</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G28">
         <v>387</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.3">

</xml_diff>